<commit_message>
Update data, comment sources
</commit_message>
<xml_diff>
--- a/app/COVID19master/data/states_beta.xlsx
+++ b/app/COVID19master/data/states_beta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Box/COVID19/UMass Analysis/COVID_sim_UMASS/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Documents/GitHub/COVID-University/app/COVID19master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63B423C-FEF5-B14C-9661-1F9159F71C9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C3EFBC-DCA1-1949-86BF-50ECC2BFF5B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11700" yWindow="7540" windowWidth="16200" windowHeight="10460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,10 +634,10 @@
         <v>0.01</v>
       </c>
       <c r="D26">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>1.4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>